<commit_message>
triggers done, some documentation
</commit_message>
<xml_diff>
--- a/Project_TimeLine_2021_07_Jan.xlsx
+++ b/Project_TimeLine_2021_07_Jan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\lms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE695ED-9FF6-4F1C-83ED-80F8BE3B4832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763D3D75-7E9F-4B6E-BDA6-0BB08F6920CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>S/N</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Identification of groups/zones/triggers</t>
+  </si>
+  <si>
+    <t>Documentation for JSON data</t>
+  </si>
+  <si>
+    <t>Documentation for existing/planned features</t>
   </si>
 </sst>
 </file>
@@ -453,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,13 +563,16 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>44203</v>
       </c>
       <c r="F4" s="3">
-        <v>44208</v>
+        <v>44203</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44203</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -577,13 +586,44 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
+        <v>44204</v>
+      </c>
+      <c r="F5" s="3">
         <v>44209</v>
       </c>
-      <c r="F5" s="3">
-        <v>44211</v>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44210</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>